<commit_message>
447	Add parameter max_trials = num_cities
</commit_message>
<xml_diff>
--- a/npbenchmark-main/travel_thief/LKH-origin/ttp运行结果.xlsx
+++ b/npbenchmark-main/travel_thief/LKH-origin/ttp运行结果.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\npbenchmark\npbenchmark-main\travel_thief\LKH-origin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAE498C0-AED3-44A9-B6D2-27B6EE5CE395}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90AD34BE-852F-4EDA-8FC8-54ED7732C4A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="32">
   <si>
     <t>object value</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -141,6 +141,10 @@
   </si>
   <si>
     <t>时间太长了</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>num_cities/2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -684,7 +688,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -835,6 +839,23 @@
         <v>27</v>
       </c>
     </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7" t="s">
+        <v>27</v>
+      </c>
+    </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>29</v>
@@ -878,5 +899,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>